<commit_message>
feat: update domain_specific_datasets.xlsx with curated datasets and metadata
</commit_message>
<xml_diff>
--- a/domain_specific_datasets.xlsx
+++ b/domain_specific_datasets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugay Talha İçen\Desktop\GitHub\Voice-To-Report-Domain-Spesific-Rag-Solition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugay Talha İçen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A03E4B-44C2-407D-8B58-E16DEB82E119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB85A2-4570-453C-9498-62A18EA04F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
-  <si>
-    <t>Dataset/Source Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="121">
+  <si>
+    <t>Dataset Name</t>
   </si>
   <si>
     <t>Domain</t>
@@ -40,19 +40,19 @@
     <t>Accessibility / License</t>
   </si>
   <si>
-    <t>Medical Speech, Transcription, and Intent</t>
-  </si>
-  <si>
-    <t>MTSamples – Medical Transcriptions</t>
-  </si>
-  <si>
-    <t>Eye Gaze Chest X-rays (EGD-CXR)</t>
-  </si>
-  <si>
-    <t>Bridge2AI Voice</t>
-  </si>
-  <si>
-    <t>MIMIC-CXR Radiology Reports</t>
+    <t>Medical Speech, Transcription, and Intent (Kaggle)</t>
+  </si>
+  <si>
+    <t>MTSamples – Medical Transcriptions (Kaggle)</t>
+  </si>
+  <si>
+    <t>Eye Gaze Chest X-rays (PhysioNet)</t>
+  </si>
+  <si>
+    <t>Bridge2AI Voice (PhysioNet)</t>
+  </si>
+  <si>
+    <t>MIMIC-CXR Radiology Reports (PhysioNet)</t>
   </si>
   <si>
     <t>Oyez Supreme Court Oral Arguments</t>
@@ -61,7 +61,7 @@
     <t>ATCOSIM Air Traffic Control Corpus</t>
   </si>
   <si>
-    <t>Apollo Fearless Steps Corpus</t>
+    <t>Apollo 'Fearless Steps' Corpus</t>
   </si>
   <si>
     <t>SPGISpeech Financial Corpus</t>
@@ -73,16 +73,40 @@
     <t>TED-LIUM (Release 3)</t>
   </si>
   <si>
-    <t>MediaSum (NPR/CNN Interviews)</t>
-  </si>
-  <si>
-    <t>Simulated Doctor-Patient Conversations</t>
+    <t>MediaSum (NPR/CNN Interview Transcripts)</t>
+  </si>
+  <si>
+    <t>Simulated Doctor-Patient Conversations (Kaggle)</t>
   </si>
   <si>
     <t>How2 – Instructional Videos Corpus</t>
   </si>
   <si>
-    <t>Mozilla Common Voice</t>
+    <t>Mozilla Common Voice (English)</t>
+  </si>
+  <si>
+    <t>LibriSpeech ASR Corpus</t>
+  </si>
+  <si>
+    <t>Open-I Chest X-ray (Indiana University)</t>
+  </si>
+  <si>
+    <t>GigaSpeech (Audio-Text Corpus)</t>
+  </si>
+  <si>
+    <t>Switchboard-1 Telephone Speech Corpus</t>
+  </si>
+  <si>
+    <t>Fisher English Training Speech Part 1</t>
+  </si>
+  <si>
+    <t>NPR Media Dialog Transcripts</t>
+  </si>
+  <si>
+    <t>LJ Speech Dataset</t>
+  </si>
+  <si>
+    <t>Medical Conversation Dataset (MedDialog-US)</t>
   </si>
   <si>
     <t>Medical – Symptoms</t>
@@ -103,13 +127,13 @@
     <t>Aviation – ATC</t>
   </si>
   <si>
-    <t>Aerospace – Mission Logs</t>
-  </si>
-  <si>
-    <t>Business – Finance Calls</t>
-  </si>
-  <si>
-    <t>Business – Meetings (Design)</t>
+    <t>Aerospace – NASA Mission Audio</t>
+  </si>
+  <si>
+    <t>Business – Finance</t>
+  </si>
+  <si>
+    <t>Business – Meetings</t>
   </si>
   <si>
     <t>Education – Presentations</t>
@@ -121,12 +145,30 @@
     <t>Medical – Clinical Dialogue</t>
   </si>
   <si>
-    <t>Education – Tutorials</t>
+    <t>Education – How-To Tutorials</t>
   </si>
   <si>
     <t>General – Crowdsourced Speech</t>
   </si>
   <si>
+    <t>General – Audiobook Narration</t>
+  </si>
+  <si>
+    <t>Multi-domain – Media, Education, Audiobooks</t>
+  </si>
+  <si>
+    <t>General – Telephone Conversations</t>
+  </si>
+  <si>
+    <t>Journalism – Radio Interviews</t>
+  </si>
+  <si>
+    <t>Education – Audiobook Reading</t>
+  </si>
+  <si>
+    <t>Medical – Doctor-Patient Dialogues</t>
+  </si>
+  <si>
     <t>https://www.kaggle.com/datasets/paultimothymooney/medical-speech-transcription-and-intent</t>
   </si>
   <si>
@@ -172,100 +214,175 @@
     <t>https://commonvoice.mozilla.org/en/datasets</t>
   </si>
   <si>
-    <t>Audio + Text</t>
-  </si>
-  <si>
-    <t>Text-only Structured Dictation</t>
-  </si>
-  <si>
-    <t>Audio + Text (partial)</t>
-  </si>
-  <si>
-    <t>Crowdsourced audio describing medical symptoms with transcripts.</t>
-  </si>
-  <si>
-    <t>5,000+ clinical notes across medical specialties.</t>
-  </si>
-  <si>
-    <t>Radiologist dictation audio with transcripts for chest X-rays.</t>
-  </si>
-  <si>
-    <t>Clinical voice samples linked to health data.</t>
-  </si>
-  <si>
-    <t>Radiologist reports for chest X-rays.</t>
-  </si>
-  <si>
-    <t>US Supreme Court oral argument audio with transcripts.</t>
-  </si>
-  <si>
-    <t>Simulated ATC speech with transcripts.</t>
-  </si>
-  <si>
-    <t>NASA Apollo mission audio with transcripts.</t>
-  </si>
-  <si>
-    <t>Earnings call audio with professional transcripts.</t>
-  </si>
-  <si>
-    <t>Meeting recordings with annotations and transcripts.</t>
-  </si>
-  <si>
-    <t>Audio from TED Talks with transcripts.</t>
-  </si>
-  <si>
-    <t>Media interview transcripts from NPR/CNN.</t>
-  </si>
-  <si>
-    <t>Synthetic clinical consultations audio.</t>
-  </si>
-  <si>
-    <t>Instructional video audio with transcripts.</t>
-  </si>
-  <si>
-    <t>Crowdsourced spoken sentences audio/transcripts.</t>
-  </si>
-  <si>
-    <t>Open (CC BY-NC)</t>
-  </si>
-  <si>
-    <t>Open (Public domain samples)</t>
-  </si>
-  <si>
-    <t>Restricted (Credentialed Research-only)</t>
-  </si>
-  <si>
-    <t>Restricted (Registered ethical use)</t>
-  </si>
-  <si>
-    <t>Open (Credentialed Research-only)</t>
-  </si>
-  <si>
-    <t>Open (Public domain)</t>
-  </si>
-  <si>
-    <t>Open (Research license)</t>
-  </si>
-  <si>
-    <t>Semi-open (IEEE DataPort)</t>
-  </si>
-  <si>
-    <t>Open (Registration, CC BY-NC)</t>
-  </si>
-  <si>
-    <t>Open (CC BY 4.0)</t>
-  </si>
-  <si>
-    <t>Open (MIT License)</t>
-  </si>
-  <si>
-    <t>Open (CC License)</t>
-  </si>
-  <si>
-    <t>Open (Creative Commons)</t>
-  </si>
-  <si>
-    <t>Open (CC0 Public Domain)</t>
+    <t>https://www.openslr.org/12</t>
+  </si>
+  <si>
+    <t>https://openi.nlm.nih.gov/</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/speechcolab/gigaspeech</t>
+  </si>
+  <si>
+    <t>https://catalog.ldc.upenn.edu/LDC97S62</t>
+  </si>
+  <si>
+    <t>https://catalog.ldc.upenn.edu/LDC2004S13</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets/shuyangli94/interview-npr-media-dialog-transcripts</t>
+  </si>
+  <si>
+    <t>https://keithito.com/LJ-Speech-Dataset/</t>
+  </si>
+  <si>
+    <t>https://github.com/UCSD-AI4H/Medical-Dialogue-System</t>
+  </si>
+  <si>
+    <t>✅ Audio + Text Paired Data</t>
+  </si>
+  <si>
+    <t>⚠️ Text-only Structured Dictation-Style</t>
+  </si>
+  <si>
+    <t>✅ Audio + Text Paired Data (partial)</t>
+  </si>
+  <si>
+    <t>8.5 hours of crowdsourced audio of people describing common medical symptoms (e.g. 'my knee hurts') with corresponding transcripts. Useful for training medical conversational agents; created via Figure-Eight platform tasks. [Kaggle](https://www.kaggle.com/datasets/paultimothymooney/medical-speech-transcription-and-intent)</t>
+  </si>
+  <si>
+    <t>5,000+ real clinical note samples across various specialties (from mtsamples.com). Contains dictated medical reports (e.g. surgical, radiology, consult notes) useful for NLP tasks in clinical domains. [Kaggle](https://www.kaggle.com/datasets/tboyle10/medicaltranscriptions)</t>
+  </si>
+  <si>
+    <t>Multimodal dataset of 1,083 chest X-rays with radiologist dictation audio and aligned transcripts. Includes the spoken report for each image (manually corrected transcripts) plus radiologist eye-tracking data for research. [PhysioNet](https://physionet.org/content/egd-cxr/1.0.0/)</t>
+  </si>
+  <si>
+    <t>Large-scale 'Voice as a Biomarker of Health' corpus (NIH Bridge2AI initiative) linking diverse voice recordings to health data. Collects ethically-sourced clinical voice samples to aid screening and diagnosis via voice analysis. [PhysioNet](https://physionet.org/content/b2ai-voice/)</t>
+  </si>
+  <si>
+    <t>377,110 chest X-ray images paired with free-text radiologist reports. Reports describe imaging findings and impressions – a rich corpus reflecting radiology dictations. [PhysioNet](https://physionet.org/content/mimic-cxr)</t>
+  </si>
+  <si>
+    <t>5,000+ hours of U.S. Supreme Court oral argument audio with transcripts. Covers ~8,000 arguments (1955–2019) with speaker-attributed transcripts. [Oyez](https://www.oyez.org/)</t>
+  </si>
+  <si>
+    <t>10 hours of simulated air traffic control operator speech by professionals, with orthographic transcripts. Includes speaker/session metadata. [HuggingFace](https://huggingface.co/datasets/Jzuluaga/atcosim_corpus)</t>
+  </si>
+  <si>
+    <t>Massive naturalistic audio from NASA Apollo missions (150,000+ hours). 19,000 hours released for community use. Partial transcripts available for ASR research. [IEEE DataPort](https://ieee-dataport.org/documents/fearless-steps-apollo-11-landing-audio)</t>
+  </si>
+  <si>
+    <t>5,000 hours of English earnings call audio from global companies with professional transcripts. Covers accents and financial terminology. [Kensho](https://datasets.kensho.com/datasets/spgispeech)</t>
+  </si>
+  <si>
+    <t>100 hours of multi-party meeting recordings (real and scenario-based) with transcripts and dialog annotations. [AMI Corpus](http://groups.inf.ed.ac.uk/ami/corpus/)</t>
+  </si>
+  <si>
+    <t>452 hours of public speaking content from TED Talks with aligned transcripts. Diverse topics and high-quality speech. [OpenSLR](https://www.openslr.org/51)</t>
+  </si>
+  <si>
+    <t>463,600 interview transcripts from NPR and CNN talk shows. Multi-turn dialogues and summaries. [HuggingFace](https://huggingface.co/datasets/nbroad/mediasum)</t>
+  </si>
+  <si>
+    <t>Approx. 1,000 simulated consultations with audio and transcripts mimicking doctor-patient discussions. [Kaggle](https://www.kaggle.com/datasets/azmayensabil/doctor-patient-conversation-large)</t>
+  </si>
+  <si>
+    <t>Around 300 hours of instructional English YouTube videos (13,500 clips) with transcriptions and translations. Covers cooking, DIY, and technical tutorials. [GitHub](https://github.com/srvk/how2-dataset)</t>
+  </si>
+  <si>
+    <t>Over 2,000 hours of English voice clips from volunteers with transcripts. Multilingual, diverse accents, public domain. [Common Voice](https://commonvoice.mozilla.org/en/datasets)</t>
+  </si>
+  <si>
+    <t>Approx. 1,000 hours of read speech from LibriVox audiobooks with exact transcripts. Public domain literature, useful for voice model pre-training. [OpenSLR](https://www.openslr.org/12)</t>
+  </si>
+  <si>
+    <t>3,955 radiology reports paired with 7,470 X-ray images. Structured clinical language used for describing findings and impressions. [NIH OpenI](https://openi.nlm.nih.gov/)</t>
+  </si>
+  <si>
+    <t>10,000 hours of English speech from podcasts, talk shows, audiobooks, and lectures. Manual transcripts included. [HuggingFace](https://huggingface.co/datasets/speechcolab/gigaspeech)</t>
+  </si>
+  <si>
+    <t>2,400 spontaneous telephone conversations (about 260 hours) between 500+ U.S. English speakers on random topics. Includes orthographic transcripts. [LDC Catalog](https://catalog.ldc.upenn.edu/LDC97S62)</t>
+  </si>
+  <si>
+    <t>5,850 telephone conversations (~585 hours) between strangers on preselected topics. Designed for large-vocabulary conversational speech recognition. [LDC Catalog](https://catalog.ldc.upenn.edu/LDC2004S13)</t>
+  </si>
+  <si>
+    <t>140,000+ transcripts from U.S. National Public Radio programs. Dialogues from shows like Fresh Air, used for summarization and QA tasks. [Kaggle](https://www.kaggle.com/datasets/shuyangli94/interview-npr-media-dialog-transcripts)</t>
+  </si>
+  <si>
+    <t>13,100 short audio clips (~24 hours) of a single speaker reading non-fiction books. Often used for TTS model training. [LJ Speech](https://keithito.com/LJ-Speech-Dataset/)</t>
+  </si>
+  <si>
+    <t>226,000+ doctor-patient dialogues across multiple medical conditions in the U.S. context. Clean, well-structured QA format. [GitHub](https://github.com/UCSD-AI4H/Medical-Dialogue-System)</t>
+  </si>
+  <si>
+    <t>Open (Kaggle) – CC BY-NC License. Requires Kaggle account to access. [License Info](https://www.kaggle.com/datasets/paultimothymooney/medical-speech-transcription-and-intent)</t>
+  </si>
+  <si>
+    <t>Open (Kaggle) – Public sample notes. [License Info](https://www.kaggle.com/datasets/tboyle10/medicaltranscriptions)</t>
+  </si>
+  <si>
+    <t>Restricted (PhysioNet) – Credentialed access required for research use. [License Info](https://physionet.org/content/egd-cxr/1.0.0/)</t>
+  </si>
+  <si>
+    <t>Restricted (PhysioNet) – Registration required; intended for ethical research use. [License Info](https://physionet.org/content/b2ai-voice/)</t>
+  </si>
+  <si>
+    <t>Open (PhysioNet) – Registration and credentialed research agreement required. [License Info](https://physionet.org/content/mimic-cxr)</t>
+  </si>
+  <si>
+    <t>Open – Public domain (via Oyez archive). [License Info](https://www.oyez.org/)</t>
+  </si>
+  <si>
+    <t>Open – Research license via TU Graz/EUROCONTROL. [License Info](https://huggingface.co/datasets/Jzuluaga/atcosim_corpus)</t>
+  </si>
+  <si>
+    <t>Semi-open – Requires approval from CRSS, UTD. [License Info](https://ieee-dataport.org/documents/fearless-steps-apollo-11-landing-audio)</t>
+  </si>
+  <si>
+    <t>Open for research – CC BY-NC License. [License Info](https://datasets.kensho.com/datasets/spgispeech)</t>
+  </si>
+  <si>
+    <t>Open – CC BY 4.0 license. [License Info](http://groups.inf.ed.ac.uk/ami/corpus/)</t>
+  </si>
+  <si>
+    <t>Open – Creative Commons BY-NC. [License Info](https://www.openslr.org/51)</t>
+  </si>
+  <si>
+    <t>Open – MIT License. [License Info](https://huggingface.co/datasets/nbroad/mediasum)</t>
+  </si>
+  <si>
+    <t>Open – CC license (synthetic data, no PHI). [License Info](https://www.kaggle.com/datasets/azmayensabil/doctor-patient-conversation-large)</t>
+  </si>
+  <si>
+    <t>Open – Creative Commons (via YouTube transcripts). [License Info](https://github.com/srvk/how2-dataset)</t>
+  </si>
+  <si>
+    <t>Open – CC0 Public Domain. [License Info](https://commonvoice.mozilla.org/en/datasets)</t>
+  </si>
+  <si>
+    <t>Open – Public domain audio (LibriVox). [License Info](https://www.openslr.org/12)</t>
+  </si>
+  <si>
+    <t>Open – NIH dataset from public repositories. [License Info](https://openi.nlm.nih.gov/faq.php)</t>
+  </si>
+  <si>
+    <t>Open – Apache 2.0 License. [License Info](https://huggingface.co/datasets/speechcolab/gigaspeech)</t>
+  </si>
+  <si>
+    <t>Restricted – Available via Linguistic Data Consortium (LDC) with academic membership. [License Info](https://catalog.ldc.upenn.edu/LDC97S62)</t>
+  </si>
+  <si>
+    <t>Restricted – Requires LDC membership or purchase. [License Info](https://catalog.ldc.upenn.edu/LDC2004S13)</t>
+  </si>
+  <si>
+    <t>Open – Transcripts scraped from NPR.org for academic use. [License Info](https://www.kaggle.com/datasets/shuyangli94/interview-npr-media-dialog-transcripts)</t>
+  </si>
+  <si>
+    <t>Open – CC BY 4.0 License. [License Info](https://keithito.com/LJ-Speech-Dataset/)</t>
+  </si>
+  <si>
+    <t>Open – Released by UCSD AI4H group. [License Info](https://github.com/UCSD-AI4H/Medical-Dialogue-System)</t>
   </si>
 </sst>
 </file>
@@ -335,12 +452,18 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -646,19 +769,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="5" max="5" width="82.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,304 +805,464 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
-        <v>81</v>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -998,6 +1282,14 @@
     <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add alternative source for MIMIC-CXR to domain_specific_datasets.xlsx
</commit_message>
<xml_diff>
--- a/domain_specific_datasets.xlsx
+++ b/domain_specific_datasets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugay Talha İçen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugay Talha İçen\Desktop\GitHub\Voice-To-Report-Domain-Spesific-Rag-Solition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB85A2-4570-453C-9498-62A18EA04F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF556CA6-A0D6-47BE-A8D3-AE8CE692C2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="122">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>Open – Released by UCSD AI4H group. [License Info](https://github.com/UCSD-AI4H/Medical-Dialogue-System)</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/code/yousefalbasel/auto-diagnostic-reports-generation-on-mimic-cxr-cn</t>
   </si>
 </sst>
 </file>
@@ -769,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +788,7 @@
     <col min="6" max="6" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -825,7 +828,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -845,7 +848,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -865,7 +868,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -885,7 +888,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -904,8 +907,11 @@
       <c r="F6" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -925,7 +931,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -945,7 +951,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -965,7 +971,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -985,7 +991,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1045,7 +1051,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1290,7 +1296,9 @@
     <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G6" r:id="rId24" xr:uid="{CBD2A86A-D1F1-4B38-BBED-A62B8257A2BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update domain_specific_datasets.xlsx for project-specific usability
</commit_message>
<xml_diff>
--- a/domain_specific_datasets.xlsx
+++ b/domain_specific_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugay Talha İçen\Desktop\GitHub\Voice-To-Report-Domain-Spesific-Rag-Solition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF556CA6-A0D6-47BE-A8D3-AE8CE692C2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87784584-A2DA-422D-8C4D-BEC66A9DABEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,12 +416,42 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -455,7 +485,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -467,6 +497,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -474,6 +509,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -775,7 +815,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +849,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -829,7 +869,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -849,7 +889,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -869,7 +909,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -889,7 +929,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
@@ -912,7 +952,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
@@ -932,7 +972,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
@@ -952,7 +992,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
@@ -972,7 +1012,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
@@ -992,7 +1032,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
@@ -1012,7 +1052,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
@@ -1032,7 +1072,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
@@ -1052,7 +1092,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
@@ -1072,7 +1112,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
@@ -1092,7 +1132,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
@@ -1112,7 +1152,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
@@ -1132,7 +1172,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
@@ -1152,7 +1192,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
@@ -1172,7 +1212,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
@@ -1192,7 +1232,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
@@ -1212,7 +1252,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
@@ -1232,7 +1272,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
@@ -1252,7 +1292,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B24" t="s">

</xml_diff>